<commit_message>
added Discount Group Consumables column to template
</commit_message>
<xml_diff>
--- a/reports/line_level_asset_report/templates/xlsx/template.xlsx
+++ b/reports/line_level_asset_report/templates/xlsx/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eklokova\code\my_connect_reports\reports\line_level_asset_report\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96560FFB-695D-48ED-8315-913C7642C368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DDD95D-896E-46E0-9F55-324916B7BBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AS$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AT$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Asset Id</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>QUANTITY</t>
+  </si>
+  <si>
+    <t>Discount Group Consumables</t>
   </si>
 </sst>
 </file>
@@ -521,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS1"/>
+  <dimension ref="A1:AT1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AQ5" sqref="AQ5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,27 +551,27 @@
     <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.42578125" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" customWidth="1"/>
-    <col min="21" max="21" width="10.28515625" customWidth="1"/>
-    <col min="22" max="22" width="13.28515625" customWidth="1"/>
-    <col min="23" max="23" width="15.28515625" customWidth="1"/>
-    <col min="24" max="24" width="18.28515625" customWidth="1"/>
-    <col min="25" max="25" width="19.85546875" customWidth="1"/>
-    <col min="26" max="27" width="17.140625" customWidth="1"/>
-    <col min="28" max="28" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="23.140625" customWidth="1"/>
-    <col min="33" max="33" width="11.42578125" customWidth="1"/>
-    <col min="34" max="34" width="11" customWidth="1"/>
-    <col min="35" max="35" width="13.7109375" customWidth="1"/>
-    <col min="36" max="36" width="10.85546875" customWidth="1"/>
-    <col min="37" max="37" width="10" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" customWidth="1"/>
-    <col min="39" max="39" width="16.7109375" customWidth="1"/>
-    <col min="40" max="40" width="13.28515625" customWidth="1"/>
+    <col min="20" max="21" width="14.85546875" customWidth="1"/>
+    <col min="22" max="22" width="10.28515625" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" customWidth="1"/>
+    <col min="24" max="24" width="15.28515625" customWidth="1"/>
+    <col min="25" max="25" width="18.28515625" customWidth="1"/>
+    <col min="26" max="26" width="19.85546875" customWidth="1"/>
+    <col min="27" max="28" width="17.140625" customWidth="1"/>
+    <col min="29" max="29" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="23.140625" customWidth="1"/>
+    <col min="34" max="34" width="11.42578125" customWidth="1"/>
+    <col min="35" max="35" width="11" customWidth="1"/>
+    <col min="36" max="36" width="13.7109375" customWidth="1"/>
+    <col min="37" max="37" width="10.85546875" customWidth="1"/>
+    <col min="38" max="38" width="10" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" customWidth="1"/>
+    <col min="40" max="40" width="16.7109375" customWidth="1"/>
+    <col min="41" max="41" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,83 +633,86 @@
         <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AT1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added HVD code to line level asset report and approved requests report
</commit_message>
<xml_diff>
--- a/reports/line_level_asset_report/templates/xlsx/template.xlsx
+++ b/reports/line_level_asset_report/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eklokova\code\my_connect_reports\reports\line_level_asset_report\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DDD95D-896E-46E0-9F55-324916B7BBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CB42E2-F9D3-4BB6-827E-39490F48492E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1305" yWindow="4305" windowWidth="21600" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AT$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AW$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Asset Id</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Discount Group Consumables</t>
+  </si>
+  <si>
+    <t>Autorenewal status</t>
+  </si>
+  <si>
+    <t>Global Sales</t>
+  </si>
+  <si>
+    <t>HVD code</t>
   </si>
 </sst>
 </file>
@@ -524,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT1"/>
+  <dimension ref="A1:AW1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AK1" sqref="AK1:AK1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,25 +562,26 @@
     <col min="19" max="19" width="13.42578125" customWidth="1"/>
     <col min="20" max="21" width="14.85546875" customWidth="1"/>
     <col min="22" max="22" width="10.28515625" customWidth="1"/>
-    <col min="23" max="23" width="13.28515625" customWidth="1"/>
-    <col min="24" max="24" width="15.28515625" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" customWidth="1"/>
-    <col min="26" max="26" width="19.85546875" customWidth="1"/>
-    <col min="27" max="28" width="17.140625" customWidth="1"/>
-    <col min="29" max="29" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="23.140625" customWidth="1"/>
-    <col min="34" max="34" width="11.42578125" customWidth="1"/>
-    <col min="35" max="35" width="11" customWidth="1"/>
-    <col min="36" max="36" width="13.7109375" customWidth="1"/>
-    <col min="37" max="37" width="10.85546875" customWidth="1"/>
-    <col min="38" max="38" width="10" customWidth="1"/>
+    <col min="23" max="23" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" customWidth="1"/>
+    <col min="26" max="26" width="18.28515625" customWidth="1"/>
+    <col min="27" max="27" width="19.85546875" customWidth="1"/>
+    <col min="28" max="29" width="17.140625" customWidth="1"/>
+    <col min="30" max="30" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="36" width="23.140625" customWidth="1"/>
+    <col min="37" max="37" width="11.42578125" customWidth="1"/>
+    <col min="38" max="38" width="11" customWidth="1"/>
     <col min="39" max="39" width="13.7109375" customWidth="1"/>
-    <col min="40" max="40" width="16.7109375" customWidth="1"/>
-    <col min="41" max="41" width="13.28515625" customWidth="1"/>
+    <col min="40" max="40" width="10.85546875" customWidth="1"/>
+    <col min="41" max="41" width="10" customWidth="1"/>
+    <col min="42" max="42" width="13.7109375" customWidth="1"/>
+    <col min="43" max="43" width="16.7109375" customWidth="1"/>
+    <col min="44" max="44" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -639,80 +649,89 @@
         <v>19</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AT1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AW1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>